<commit_message>
#ES-303 - updated evaluation-logs-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
+++ b/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
@@ -38,7 +38,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:area(lastCell="L8")</t>
+          <t>jx:area(lastCell="M8")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="L3", areas=["A3:B3"])</t>
+          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="M3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -88,7 +88,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.filters" var="filter" lastCell="L4")</t>
+          <t>jx:each(items="report.filters" var="filter" lastCell="M4")</t>
         </r>
       </text>
     </comment>
@@ -113,7 +113,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.items" var="evaluationLog" lastCell="L7")</t>
+          <t>jx:each(items="report.items" var="evaluationLog" lastCell="M7")</t>
         </r>
       </text>
     </comment>
@@ -157,6 +157,9 @@
     <t>Метод оценки точности</t>
   </si>
   <si>
+    <t>Пользователь</t>
+  </si>
+  <si>
     <t>Модель классификатора</t>
   </si>
   <si>
@@ -206,6 +209,16 @@
   </si>
   <si>
     <t>${evaluationLog.evaluationMethod}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${evaluationLog.createdBy}</t>
+    </r>
   </si>
   <si>
     <r>
@@ -605,7 +618,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:AMN8"/>
+  <dimension ref="A1:AMO8"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -615,17 +628,17 @@
     <col customWidth="true" max="2" min="2" outlineLevel="0" width="40.2187508193987"/>
     <col customWidth="true" max="3" min="3" outlineLevel="0" width="31.8867182048355"/>
     <col customWidth="true" max="5" min="4" outlineLevel="0" width="37.8867178665032"/>
-    <col customWidth="true" max="6" min="6" outlineLevel="0" width="38.664062184135"/>
-    <col customWidth="true" hidden="false" max="7" min="7" outlineLevel="0" width="58.4315906340805"/>
-    <col customWidth="true" max="9" min="8" outlineLevel="0" width="32.3320312612337"/>
-    <col customWidth="true" max="10" min="10" outlineLevel="0" width="51.8867161748414"/>
-    <col customWidth="true" max="12" min="11" outlineLevel="0" width="57.7773424568038"/>
-    <col customWidth="true" max="13" min="13" outlineLevel="0" width="26.9999998308338"/>
-    <col customWidth="true" max="14" min="14" outlineLevel="0" width="30.8867187123341"/>
-    <col customWidth="true" max="15" min="15" outlineLevel="0" width="34.3320302462366"/>
-    <col customWidth="true" max="16" min="16" outlineLevel="0" width="31.4414051484374"/>
-    <col customWidth="true" max="17" min="17" outlineLevel="0" width="31.5546869436019"/>
-    <col customWidth="true" max="1028" min="18" outlineLevel="0" width="8.55468778943276"/>
+    <col customWidth="true" max="7" min="6" outlineLevel="0" width="38.664062184135"/>
+    <col customWidth="true" hidden="false" max="8" min="8" outlineLevel="0" width="58.4315906340805"/>
+    <col customWidth="true" max="10" min="9" outlineLevel="0" width="32.3320312612337"/>
+    <col customWidth="true" max="11" min="11" outlineLevel="0" width="51.8867161748414"/>
+    <col customWidth="true" max="13" min="12" outlineLevel="0" width="57.7773424568038"/>
+    <col customWidth="true" max="14" min="14" outlineLevel="0" width="26.9999998308338"/>
+    <col customWidth="true" max="15" min="15" outlineLevel="0" width="30.8867187123341"/>
+    <col customWidth="true" max="16" min="16" outlineLevel="0" width="34.3320302462366"/>
+    <col customWidth="true" max="17" min="17" outlineLevel="0" width="31.4414051484374"/>
+    <col customWidth="true" max="18" min="18" outlineLevel="0" width="31.5546869436019"/>
+    <col customWidth="true" max="1029" min="19" outlineLevel="0" width="8.55468778943276"/>
   </cols>
   <sheetData>
     <row ht="15.6000003814697" outlineLevel="0" r="1">
@@ -643,11 +656,12 @@
       <c r="J1" s="1" t="s"/>
       <c r="K1" s="1" t="s"/>
       <c r="L1" s="1" t="s"/>
-      <c r="M1" s="0" t="n"/>
+      <c r="M1" s="1" t="s"/>
       <c r="N1" s="0" t="n"/>
       <c r="O1" s="0" t="n"/>
       <c r="P1" s="0" t="n"/>
       <c r="Q1" s="0" t="n"/>
+      <c r="R1" s="0" t="n"/>
     </row>
     <row ht="15.6000003814697" outlineLevel="0" r="2">
       <c r="A2" s="2" t="n"/>
@@ -662,11 +676,12 @@
       <c r="J2" s="3" t="n"/>
       <c r="K2" s="3" t="n"/>
       <c r="L2" s="3" t="n"/>
-      <c r="M2" s="0" t="n"/>
+      <c r="M2" s="3" t="n"/>
       <c r="N2" s="0" t="n"/>
       <c r="O2" s="0" t="n"/>
       <c r="P2" s="0" t="n"/>
       <c r="Q2" s="0" t="n"/>
+      <c r="R2" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
@@ -685,11 +700,12 @@
       <c r="J3" s="5" t="s"/>
       <c r="K3" s="5" t="s"/>
       <c r="L3" s="5" t="s"/>
-      <c r="M3" s="0" t="n"/>
+      <c r="M3" s="5" t="s"/>
       <c r="N3" s="0" t="n"/>
       <c r="O3" s="0" t="n"/>
       <c r="P3" s="0" t="n"/>
       <c r="Q3" s="0" t="n"/>
+      <c r="R3" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
@@ -708,11 +724,12 @@
       <c r="J4" s="5" t="s"/>
       <c r="K4" s="5" t="s"/>
       <c r="L4" s="5" t="s"/>
-      <c r="M4" s="0" t="n"/>
+      <c r="M4" s="5" t="s"/>
       <c r="N4" s="0" t="n"/>
       <c r="O4" s="0" t="n"/>
       <c r="P4" s="0" t="n"/>
       <c r="Q4" s="0" t="n"/>
+      <c r="R4" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="3" t="n"/>
@@ -727,11 +744,12 @@
       <c r="J5" s="3" t="n"/>
       <c r="K5" s="3" t="n"/>
       <c r="L5" s="3" t="n"/>
-      <c r="M5" s="0" t="n"/>
+      <c r="M5" s="3" t="n"/>
       <c r="N5" s="0" t="n"/>
       <c r="O5" s="0" t="n"/>
       <c r="P5" s="0" t="n"/>
       <c r="Q5" s="0" t="n"/>
+      <c r="R5" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="7" t="s">
@@ -761,67 +779,73 @@
       <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="9" t="n"/>
+      <c r="M6" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="N6" s="9" t="n"/>
       <c r="O6" s="9" t="n"/>
       <c r="P6" s="9" t="n"/>
       <c r="Q6" s="9" t="n"/>
+      <c r="R6" s="9" t="n"/>
     </row>
     <row customHeight="true" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="K7" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="L7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="0" t="n"/>
+        <v>29</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="N7" s="0" t="n"/>
       <c r="O7" s="0" t="n"/>
       <c r="P7" s="0" t="n"/>
       <c r="Q7" s="0" t="n"/>
+      <c r="R7" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="14" t="s"/>
       <c r="C8" s="14" t="s"/>
@@ -833,19 +857,20 @@
       <c r="I8" s="14" t="s"/>
       <c r="J8" s="14" t="s"/>
       <c r="K8" s="14" t="s"/>
-      <c r="L8" s="15" t="s"/>
-      <c r="M8" s="0" t="n"/>
+      <c r="L8" s="14" t="s"/>
+      <c r="M8" s="15" t="s"/>
       <c r="N8" s="0" t="n"/>
       <c r="O8" s="0" t="n"/>
       <c r="P8" s="0" t="n"/>
       <c r="Q8" s="0" t="n"/>
+      <c r="R8" s="0" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="A8:M8"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.511805534362793" header="0.511805534362793" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
   <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297mm" paperSize="9" paperWidth="210mm" scale="100"/>

</xml_diff>

<commit_message>
ECS-8 updated xls report templates
</commit_message>
<xml_diff>
--- a/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
+++ b/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
@@ -38,7 +38,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:area(lastCell="M8")</t>
+          <t>jx:area(lastCell="M10")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,16 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>Roman93:</t>
+          <t>jx:each(items="report.filters" var="filter" lastCell="M6"</t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>)</t>
         </r>
         <r>
           <t xml:space="preserve">
@@ -85,14 +94,86 @@
         <r>
           <rPr>
             <rFont val="Tahoma"/>
-            <color rgb="000000" tint="0"/>
-            <sz val="9"/>
-          </rPr>
-          <t>jx:each(items="report.filters" var="filter" lastCell="M4")</t>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>jx:if(condition="filter.filterFieldType != 'DATE' &amp;&amp; not empty(filter.value1)</t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>", lastCell="M4", areas=["A4:B4"])</t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A7">
+    <comment authorId="0" ref="A5">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t xml:space="preserve">jx:if(condition="filter.filterFieldType == 'DATE' &amp;&amp; filter.matchMode == 'RANGE' &amp;&amp; not empty(filter.value1) &amp;&amp; </t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>not empty(filter.value2)</t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>", lastCell="M5", areas=["A5:B5"])</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A6">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t xml:space="preserve">jx:if(condition="filter.filterFieldType == 'DATE' &amp;&amp; filter.matchMode == 'RANGE' &amp;&amp; not empty(filter.value1) &amp;&amp; </t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>filter.value2 == null</t>
+        </r>
+        <r>
+          <rPr>
+            <rFont val="Tahoma"/>
+            <b val="true"/>
+            <color rgb="000000" tint="0"/>
+            <sz val="9"/>
+          </rPr>
+          <t>", lastCell="M6", areas=["A6:B6"])</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A9">
       <text>
         <r>
           <rPr>
@@ -113,7 +194,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.items" var="evaluationLog" lastCell="M7")</t>
+          <t>jx:each(items="report.items" var="evaluationLog" lastCell="M9")</t>
         </r>
       </text>
     </comment>
@@ -133,10 +214,69 @@
     <t>${report.searchQuery}</t>
   </si>
   <si>
-    <t>${filter.description}</t>
-  </si>
-  <si>
-    <t>${filter.filterData}</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${filter.description}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${filter.value1}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">с </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">${filter.value1} по </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${filter.value2}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">с </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${filter.value1}</t>
+    </r>
   </si>
   <si>
     <t>UUID заявки</t>
@@ -367,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="1000" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="2" fontId="1" numFmtId="1000" quotePrefix="false"/>
     <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="3" fontId="1" numFmtId="1000" quotePrefix="false"/>
@@ -379,6 +519,7 @@
     <xf applyAlignment="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment wrapText="true"/>
     </xf>
+    <xf applyFill="true" applyFont="true" applyNumberFormat="true" borderId="0" fillId="4" fontId="0" numFmtId="1000" quotePrefix="false"/>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="5" fontId="2" numFmtId="1000" quotePrefix="false">
       <alignment horizontal="center"/>
     </xf>
@@ -618,7 +759,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:AMO8"/>
+  <dimension ref="A1:AMO10"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -711,132 +852,88 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s"/>
-      <c r="D4" s="5" t="s"/>
-      <c r="E4" s="5" t="s"/>
-      <c r="F4" s="5" t="s"/>
-      <c r="G4" s="5" t="s"/>
-      <c r="H4" s="5" t="s"/>
-      <c r="I4" s="5" t="s"/>
-      <c r="J4" s="5" t="s"/>
-      <c r="K4" s="5" t="s"/>
-      <c r="L4" s="5" t="s"/>
-      <c r="M4" s="5" t="s"/>
+      <c r="C4" s="7" t="s"/>
+      <c r="D4" s="7" t="s"/>
+      <c r="E4" s="7" t="s"/>
+      <c r="F4" s="7" t="s"/>
+      <c r="G4" s="7" t="s"/>
+      <c r="H4" s="5" t="n"/>
+      <c r="I4" s="5" t="n"/>
+      <c r="J4" s="5" t="n"/>
+      <c r="K4" s="5" t="n"/>
+      <c r="L4" s="5" t="n"/>
+      <c r="M4" s="5" t="n"/>
       <c r="N4" s="0" t="n"/>
       <c r="O4" s="0" t="n"/>
       <c r="P4" s="0" t="n"/>
       <c r="Q4" s="0" t="n"/>
       <c r="R4" s="0" t="n"/>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="3" t="n"/>
-      <c r="M5" s="3" t="n"/>
+    <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="5">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s"/>
+      <c r="D5" s="7" t="s"/>
+      <c r="E5" s="7" t="s"/>
+      <c r="F5" s="7" t="s"/>
+      <c r="G5" s="7" t="s"/>
+      <c r="H5" s="5" t="n"/>
+      <c r="I5" s="5" t="n"/>
+      <c r="J5" s="5" t="n"/>
+      <c r="K5" s="5" t="n"/>
+      <c r="L5" s="5" t="n"/>
+      <c r="M5" s="5" t="n"/>
       <c r="N5" s="0" t="n"/>
       <c r="O5" s="0" t="n"/>
       <c r="P5" s="0" t="n"/>
       <c r="Q5" s="0" t="n"/>
       <c r="R5" s="0" t="n"/>
     </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
+    <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="6">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="9" t="n"/>
-      <c r="O6" s="9" t="n"/>
-      <c r="P6" s="9" t="n"/>
-      <c r="Q6" s="9" t="n"/>
-      <c r="R6" s="9" t="n"/>
+      <c r="C6" s="7" t="s"/>
+      <c r="D6" s="7" t="s"/>
+      <c r="E6" s="7" t="s"/>
+      <c r="F6" s="7" t="s"/>
+      <c r="G6" s="7" t="s"/>
+      <c r="H6" s="5" t="n"/>
+      <c r="I6" s="5" t="n"/>
+      <c r="J6" s="5" t="n"/>
+      <c r="K6" s="5" t="n"/>
+      <c r="L6" s="5" t="n"/>
+      <c r="M6" s="5" t="n"/>
+      <c r="N6" s="0" t="n"/>
+      <c r="O6" s="0" t="n"/>
+      <c r="P6" s="0" t="n"/>
+      <c r="Q6" s="0" t="n"/>
+      <c r="R6" s="0" t="n"/>
     </row>
-    <row customHeight="true" ht="15" outlineLevel="0" r="7">
-      <c r="A7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>30</v>
-      </c>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="3" t="n"/>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+      <c r="J7" s="3" t="n"/>
+      <c r="K7" s="3" t="n"/>
+      <c r="L7" s="3" t="n"/>
+      <c r="M7" s="3" t="n"/>
       <c r="N7" s="0" t="n"/>
       <c r="O7" s="0" t="n"/>
       <c r="P7" s="0" t="n"/>
@@ -844,33 +941,127 @@
       <c r="R7" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="10" t="n"/>
+      <c r="O8" s="10" t="n"/>
+      <c r="P8" s="10" t="n"/>
+      <c r="Q8" s="10" t="n"/>
+      <c r="R8" s="10" t="n"/>
+    </row>
+    <row customHeight="true" ht="15" outlineLevel="0" r="9">
+      <c r="A9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="14" t="s"/>
-      <c r="C8" s="14" t="s"/>
-      <c r="D8" s="14" t="s"/>
-      <c r="E8" s="14" t="s"/>
-      <c r="F8" s="14" t="s"/>
-      <c r="G8" s="14" t="s"/>
-      <c r="H8" s="14" t="s"/>
-      <c r="I8" s="14" t="s"/>
-      <c r="J8" s="14" t="s"/>
-      <c r="K8" s="14" t="s"/>
-      <c r="L8" s="14" t="s"/>
-      <c r="M8" s="15" t="s"/>
-      <c r="N8" s="0" t="n"/>
-      <c r="O8" s="0" t="n"/>
-      <c r="P8" s="0" t="n"/>
-      <c r="Q8" s="0" t="n"/>
-      <c r="R8" s="0" t="n"/>
+      <c r="M9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="0" t="n"/>
+      <c r="O9" s="0" t="n"/>
+      <c r="P9" s="0" t="n"/>
+      <c r="Q9" s="0" t="n"/>
+      <c r="R9" s="0" t="n"/>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="15" t="s"/>
+      <c r="C10" s="15" t="s"/>
+      <c r="D10" s="15" t="s"/>
+      <c r="E10" s="15" t="s"/>
+      <c r="F10" s="15" t="s"/>
+      <c r="G10" s="15" t="s"/>
+      <c r="H10" s="15" t="s"/>
+      <c r="I10" s="15" t="s"/>
+      <c r="J10" s="15" t="s"/>
+      <c r="K10" s="15" t="s"/>
+      <c r="L10" s="15" t="s"/>
+      <c r="M10" s="16" t="s"/>
+      <c r="N10" s="0" t="n"/>
+      <c r="O10" s="0" t="n"/>
+      <c r="P10" s="0" t="n"/>
+      <c r="Q10" s="0" t="n"/>
+      <c r="R10" s="0" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.511805534362793" header="0.511805534362793" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
   <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297mm" paperSize="9" paperWidth="210mm" scale="100"/>

</xml_diff>

<commit_message>
ECS-62 added evaluationTimeMillis field calculation
</commit_message>
<xml_diff>
--- a/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
+++ b/eca-server/src/main/resources/report-templates/evaluation-logs-report-template.xlsx
@@ -309,7 +309,7 @@
     <t>Дата создания заявки</t>
   </si>
   <si>
-    <t>Дата начала построения модели</t>
+    <t>Дата начала обработки заявки</t>
   </si>
   <si>
     <r>
@@ -319,7 +319,7 @@
         <color rgb="000000" tint="0"/>
         <sz val="11"/>
       </rPr>
-      <t>Дата окончания построения модели</t>
+      <t>Дата окончания обработки заявки</t>
     </r>
   </si>
   <si>

</xml_diff>